<commit_message>
Highlighted two additional names in the review
</commit_message>
<xml_diff>
--- a/Data/ITIS_name_review.xlsx
+++ b/Data/ITIS_name_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/frowland_usgs_gov/Documents/Documents/Repositories/crass-fish/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC2DA9CC-4475-4DFF-BBCA-3323014995AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{DC2DA9CC-4475-4DFF-BBCA-3323014995AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9F414F1-3C63-4E02-B4C0-1E6E8CF4FE52}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{2436C99E-198D-4991-B739-F2E850D978E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{2436C99E-198D-4991-B739-F2E850D978E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Common names" sheetId="1" r:id="rId1"/>
@@ -9309,7 +9309,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>537</v>
       </c>
@@ -9350,7 +9350,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>538</v>
       </c>
@@ -9391,7 +9391,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>539</v>
       </c>
@@ -9432,7 +9432,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="22.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>540</v>
       </c>
@@ -12296,8 +12296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55A7669-88EC-40FF-A071-C463782C850E}">
   <dimension ref="A1:E415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="L229" sqref="L229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13769,7 +13769,7 @@
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+      <c r="A89" s="8" t="s">
         <v>1140</v>
       </c>
       <c r="B89" t="s">
@@ -16263,7 +16263,7 @@
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A241" t="s">
+      <c r="A241" s="8" t="s">
         <v>773</v>
       </c>
       <c r="B241" t="s">

</xml_diff>

<commit_message>
Changed from Phoxinus belimiauensis to Phoxinus grumi belimiauensis
</commit_message>
<xml_diff>
--- a/Data/ITIS_name_review.xlsx
+++ b/Data/ITIS_name_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/frowland_usgs_gov/Documents/Documents/Repositories/crass-fish/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{DC2DA9CC-4475-4DFF-BBCA-3323014995AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A037BA99-F6F2-4D0F-8B07-B2078E76A152}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{DC2DA9CC-4475-4DFF-BBCA-3323014995AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B70F3351-F360-4DC2-83F5-442ECFD91E7F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{2436C99E-198D-4991-B739-F2E850D978E3}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="1" activeTab="2" xr2:uid="{2436C99E-198D-4991-B739-F2E850D978E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Common names" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3650" uniqueCount="1260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3650" uniqueCount="1259">
   <si>
     <t>commonname</t>
   </si>
@@ -3799,18 +3799,12 @@
     <t>Can't find</t>
   </si>
   <si>
-    <t>is it Phoxinus phoxinus?</t>
-  </si>
-  <si>
     <t>Rhynchocypris czekanowskii, Czekanowski's minnow (fishbase.de)</t>
   </si>
   <si>
     <t>Rhynchocypris czekanowskii</t>
   </si>
   <si>
-    <t>DELETE ROW?</t>
-  </si>
-  <si>
     <t>Rocio octofasciata, Jack Dempsey : aquarium (fishbase.de)</t>
   </si>
   <si>
@@ -3818,6 +3812,9 @@
   </si>
   <si>
     <t>Skiffia bilineata, Twoline skiffia : aquarium (fishbase.de)</t>
+  </si>
+  <si>
+    <t>Phoxinus grumi belimiauensis</t>
   </si>
 </sst>
 </file>
@@ -4298,7 +4295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D425BBB0-5327-44F8-BF95-DAC042128A38}">
   <dimension ref="A1:F415"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
@@ -9286,8 +9283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D973E6-BCCA-4232-8EB9-92AA34B843E1}">
   <dimension ref="A1:R415"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10005,7 +10002,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>549</v>
       </c>
@@ -10019,10 +10016,10 @@
         <v>1252</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>1253</v>
+        <v>1258</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>1256</v>
+        <v>970</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>1053</v>
@@ -10060,10 +10057,10 @@
         <v>965</v>
       </c>
       <c r="H18" s="6" t="s">
+        <v>1253</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>1254</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>1255</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>970</v>
@@ -10104,10 +10101,10 @@
         <v>966</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>1230</v>
@@ -10192,7 +10189,7 @@
         <v>968</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>1232</v>
@@ -12542,8 +12539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55A7669-88EC-40FF-A071-C463782C850E}">
   <dimension ref="A1:I415"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B387" sqref="B387"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13631,7 +13628,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="13" t="s">
-        <v>598</v>
+        <v>1258</v>
       </c>
       <c r="B66" t="s">
         <v>1157</v>
@@ -13648,7 +13645,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="13" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="B67" t="s">
         <v>1177</v>

</xml_diff>